<commit_message>
Rozszerz ryzyka techniczne, planowania i opłacaloności
</commit_message>
<xml_diff>
--- a/Cwiczenie-4/ryzyka.xlsx
+++ b/Cwiczenie-4/ryzyka.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="22995" windowHeight="10035" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Zbiorczy" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
   <si>
     <t>Kwalifikacje i doświadczenie członków zespołu</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Gęstość pracochłonności</t>
   </si>
   <si>
-    <t>Wiarygodność szacowania</t>
-  </si>
-  <si>
     <t>Nazwa</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>Uzasadnienie wyboru mitygacji</t>
   </si>
   <si>
-    <t>Unikanie poprzez szkolenia w fazie przygotowania do projektu</t>
-  </si>
-  <si>
     <t>Prawdopodobieństwo (1-6)</t>
   </si>
   <si>
@@ -57,81 +51,9 @@
     <t>Doświadczenie kierownika projektu</t>
   </si>
   <si>
-    <t>Dostępność zasobów</t>
-  </si>
-  <si>
     <t>Przyjęcie</t>
   </si>
   <si>
-    <t>Zmniejszenie prawdopodobieństwa poprzez regularne raporty i kontrolę postępu prac</t>
-  </si>
-  <si>
-    <t>Zmniejszenie prawdopodobieństwa poprzez wcześniejsze pozyskanie zasobów</t>
-  </si>
-  <si>
-    <t>Zmniejszenie wpływu : ustalenie podkierownictwa, mosty komunikacyjne pomiędzy kierownikiem głównym, a podkierownictwem</t>
-  </si>
-  <si>
-    <t>Niestabilność na rynku technologii mobilnych</t>
-  </si>
-  <si>
-    <t>Jednoznaczność wymagań</t>
-  </si>
-  <si>
-    <t>Zlożonośc systemu</t>
-  </si>
-  <si>
-    <t>Unikanie: rzetelna analiza i dokumentacja funkcjonalna</t>
-  </si>
-  <si>
-    <t>Zmniejszanie prawdopodobieństwa: jasne zasady architektury, wzorce projektowe</t>
-  </si>
-  <si>
-    <t>Złożoność infrastruktury komunikacyjnej</t>
-  </si>
-  <si>
-    <t>Problemy z efektywną komunikacją na płaszczyźnie aplikacja-serwer</t>
-  </si>
-  <si>
-    <t>Zmniejszenie prawdopodobieństwa: korzystanie ze sprawdzonych rozwiązań</t>
-  </si>
-  <si>
-    <t>Wydajność systemu</t>
-  </si>
-  <si>
-    <t>Zmniejszenie prawdopodobieństwa: poszukiwanie gotowych rozwiązań</t>
-  </si>
-  <si>
-    <t>Płynność kosztów</t>
-  </si>
-  <si>
-    <t>Płynnośc zakresu</t>
-  </si>
-  <si>
-    <t>Okres zwrotu inwestycji</t>
-  </si>
-  <si>
-    <t>Popracie biznesowe</t>
-  </si>
-  <si>
-    <t>Zmniejszenie wpływu: pozyskanie środków większych niż zakładany budżet</t>
-  </si>
-  <si>
-    <t>Ewentualne zmiany w zakresie podyktowane żądaniami partnerów</t>
-  </si>
-  <si>
-    <t>Delegacja: wynajęcie zewnętrznej agencji reklamowej</t>
-  </si>
-  <si>
-    <t>Zmniejszenie prawdopodobieństwa: wzmocnienie gałęzi kontaktów z partnerami</t>
-  </si>
-  <si>
-    <t>Zainteresowanie użytkowników</t>
-  </si>
-  <si>
-    <t>Zmniejszenie prawdopodobieństwa: reklama i wynegocjowanie dobrych rabatów</t>
-  </si>
-  <si>
     <t>Potrzeba edukacji</t>
   </si>
   <si>
@@ -178,33 +100,145 @@
   </si>
   <si>
     <t>Gdy ktoś nas uprzedzi - wprowadzi produkt przed nami</t>
+  </si>
+  <si>
+    <t>Plan organizacji prac nad projektem nie pozwala na duże opóźnienia między zadaniami. Ścieżka krytyczna zawiera zdecydowaną większość zadań, opóźnienie jednego może wpłynąć znacznie na opóźnienie całego projektu.</t>
+  </si>
+  <si>
+    <t>Plan organizacji projektu zakłada zarządzanie kilkoma zadaniami równolegle. W późniejszych etapach prac, manager może mieć problem z  nadzorem grupy zadań jednocześnie.</t>
+  </si>
+  <si>
+    <t>Projekt wymaga specjalistycznej wiedzy z zakresu przetwarzania obrazów. Zebranie zespołu posiadającego doświadczenie w tej dziedzinie jest nieopłacalne przy dostępnych zasobach projektu. Zespół po szkoleniu nadal może nie posiadać wystarczającej wiedzy.</t>
+  </si>
+  <si>
+    <t>Nawiązanie współpracy z konsultantem, z doświadczeniem w dziedzinie przetwarzania obrazów.</t>
+  </si>
+  <si>
+    <t>Typ mitygacji</t>
+  </si>
+  <si>
+    <t>Zmniejszanie wpływu</t>
+  </si>
+  <si>
+    <t>Zmniejszenie prawdopodobieństwa</t>
+  </si>
+  <si>
+    <t>Regularne raporty. Kontrola postępu prac. Dobranie metodyki.</t>
+  </si>
+  <si>
+    <t>Zmniejszenie wpływu</t>
+  </si>
+  <si>
+    <t>Ustalenie hierarchii kierownictwa. Protokoły komunikacyjne.</t>
+  </si>
+  <si>
+    <t>Zasadność planu biznesowego</t>
+  </si>
+  <si>
+    <t>Niewystarczające fundusze na utrzymanie projektu do czasu znalezienia inwestorów.</t>
+  </si>
+  <si>
+    <t>Kredyt.</t>
+  </si>
+  <si>
+    <t>Jak najszybsze pozyskanie inwestorów.</t>
+  </si>
+  <si>
+    <t>Dynamiczność rynku technologii mobilnych</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rynek technologii mobilnych jest podatny na zmiany. Wybrana technologia może się zdeaktualizować w bliskiej przyszłości. </t>
+  </si>
+  <si>
+    <t>Rozszerzenie zakresu produktów do kilku aplikacji mobilnych na różne platformy.</t>
+  </si>
+  <si>
+    <t>Jednoznaczność specyfikacji funkcjonalnej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niejasny opis funkcjonalności oferowanej organizatorom utrudnia nawiązanie współpracy. </t>
+  </si>
+  <si>
+    <t>Analiza przyczyn braku zainteresowania współpracą poprzez feedback od organizatorów.</t>
+  </si>
+  <si>
+    <t>Zmniejszanie prawdopodobieństwa</t>
+  </si>
+  <si>
+    <t>Stosowanie formalnej metodyki, zakładającej wykorzystanie ciągłego procesu testowania.</t>
+  </si>
+  <si>
+    <t>Złożoność systemu</t>
+  </si>
+  <si>
+    <t>Projekt techniczny zakłada rozdzielenie na kilka niezależnych modułów, które muszą współpracować. Synchronizacja rozwoju modułów i weryfikacja ich współpracy jest nietrywialne.</t>
+  </si>
+  <si>
+    <t>Sprawność operacyjna</t>
+  </si>
+  <si>
+    <t>Korzystanie ze standardów. Redundancja infrastruktury: replikacja bazy danych, wiele instancji serwerów, rozdział obciążenia.</t>
+  </si>
+  <si>
+    <t>Problemy z efektywną komunikacją między podsystemami. Trwałość i bezpieczeństwo przechowywania danych. Zachowanie uptime'u przy nieregularnych skokach obciążenia.</t>
+  </si>
+  <si>
+    <t>Poparcie biznesowe inwestorów</t>
+  </si>
+  <si>
+    <t>Realizacja iteracji C "Wdrożenie" jest niemożliwa bez wczesnego wsparcia finansowego inwestorów.</t>
+  </si>
+  <si>
+    <t>Zwiększenie nakładów na pozyskiwanie inwestorów: organizacja happeningów, efektowna prezentacja możliwości produktów.</t>
+  </si>
+  <si>
+    <t>Oferowanie korzystniejszych warunków współpracy dla pierwszej grupy inwestorów.</t>
+  </si>
+  <si>
+    <t>Eksluzywne nawiązywanie współpracy.</t>
+  </si>
+  <si>
+    <t>Przyjęcie aplikacji mobilnej przez użytkowników</t>
+  </si>
+  <si>
+    <t>Rabat przy zakupie biletów, w porozumieniu z organizatorami.</t>
+  </si>
+  <si>
+    <t>Projekt UI appki</t>
+  </si>
+  <si>
+    <t>Zmniejszenie wpłytu</t>
+  </si>
+  <si>
+    <t>Renegocjacja wysokości prowizji od sprzedaży biletów.</t>
+  </si>
+  <si>
+    <t>Elastyczność kosztów</t>
+  </si>
+  <si>
+    <t>Możliwa jest różnica kosztów projektu wynikająca z nadgodzin lub opóźnień zidentyfikowanych w innych ryzykach.</t>
+  </si>
+  <si>
+    <t>Polegamy na mitygacji ryzyk opóźniających pracę.</t>
+  </si>
+  <si>
+    <t>Elastyczność zakresu projektu</t>
+  </si>
+  <si>
+    <t>Ewentualne zmiany w zakresie projektu podyktowane żądaniami priorytetowych inwestorów.</t>
+  </si>
+  <si>
+    <t>Praca, praca, praca. Więcej pracy.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -219,26 +253,23 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -246,36 +277,30 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Check Cell" xfId="2" builtinId="23"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -587,114 +612,148 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="44.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="4">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4">
+        <v>5</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="C5" s="4">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="4">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -705,113 +764,129 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="5" customWidth="1"/>
+    <col min="4" max="5" width="26.140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="29" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="6">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3">
+      <c r="E2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="6">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="6">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
+      <c r="D4" s="6">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
+      <c r="E4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="6">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6">
+      <c r="D5" s="6">
         <v>4</v>
       </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
+      <c r="E5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -822,113 +897,146 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" customWidth="1"/>
-    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="1" max="1" width="45.5703125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="27" style="5" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="29" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="5">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="E6" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="5">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4">
+      <c r="D7" s="5">
         <v>4</v>
       </c>
-      <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E7" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
+      <c r="F7" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="E8" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -957,30 +1065,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -989,12 +1097,12 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1003,12 +1111,12 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1017,7 +1125,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1030,7 +1138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1046,27 +1154,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -1075,12 +1183,12 @@
         <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -1089,12 +1197,12 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1103,12 +1211,12 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1117,15 +1225,15 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -1134,7 +1242,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>